<commit_message>
Modelo enriquecido de Notificacion
</commit_message>
<xml_diff>
--- a/SpaOnline/ModeloDominio/Notificación - Muestreo Datos.xlsx
+++ b/SpaOnline/ModeloDominio/Notificación - Muestreo Datos.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DOO\DOO\SpaOnline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grchia-my.sharepoint.com/personal/jhonatan_gomez_wiga_io/Documents/Escritorio/UCO/DOO GIT/SpaOnline/ModeloDominio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E86E8DA-E599-4D9B-A5F4-75B54B44BEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="13_ncr:1_{7E86E8DA-E599-4D9B-A5F4-75B54B44BEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBF39B0F-394D-46E7-BDE8-ECF8F6034223}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo de Dominio Anemico" sheetId="1" r:id="rId1"/>
     <sheet name="Objetos de dominio" sheetId="2" r:id="rId2"/>
     <sheet name="Notificación" sheetId="5" r:id="rId3"/>
+    <sheet name="TipoNotificacion" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t xml:space="preserve">Nombre </t>
   </si>
@@ -72,9 +73,6 @@
     <t>Contextro</t>
   </si>
   <si>
-    <t>Fabricante</t>
-  </si>
-  <si>
     <t>Propio</t>
   </si>
   <si>
@@ -87,13 +85,43 @@
     <t>Combinacion única</t>
   </si>
   <si>
-    <t>Producto</t>
-  </si>
-  <si>
     <t>Notificación</t>
   </si>
   <si>
     <t>Objeto de dominio que contiene la informacion de las notificaciones que emite el Spa</t>
+  </si>
+  <si>
+    <t>TipoNotificacion</t>
+  </si>
+  <si>
+    <t>Servicio</t>
+  </si>
+  <si>
+    <t>Pago</t>
+  </si>
+  <si>
+    <t>Transaccional</t>
+  </si>
+  <si>
+    <t>IdPago</t>
+  </si>
+  <si>
+    <t>Objeto de dominio que contiene el tipo de notificacion que se va a enviar para la trazabildiad</t>
+  </si>
+  <si>
+    <t>Referenciado</t>
+  </si>
+  <si>
+    <t>Notificacion</t>
+  </si>
+  <si>
+    <t>Objeto de dominio que contiene el id del servicio que vamos a notificar</t>
+  </si>
+  <si>
+    <t>Objeto de dominio que contiene el id del Pago que vamos a notificar</t>
+  </si>
+  <si>
+    <t>IdServicio</t>
   </si>
 </sst>
 </file>
@@ -164,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -183,6 +211,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -205,22 +239,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>686640</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>29323</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>429513</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>153006</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{435323B5-5A53-8557-75BD-68CDE1A05E0D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C698122-2573-A5AB-7957-8B0A82AAA14D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -236,8 +270,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="6020640" cy="5363323"/>
+          <a:off x="161925" y="0"/>
+          <a:ext cx="6363588" cy="4344006"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -585,7 +619,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="P24" sqref="P23:P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,18 +634,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D92343-C7F8-498A-9249-704487594109}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="65.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -630,16 +664,58 @@
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
+      <c r="B4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -650,65 +726,127 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952BDDC5-1485-4BC4-A31B-18839936F54D}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="5" t="str">
+      <c r="B2" s="1" t="str">
+        <f>TipoNotificacion!C2</f>
+        <v>Servicio</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="10">
+        <v>0</v>
+      </c>
+      <c r="E2" s="5" t="str">
         <f>B2&amp;"-"&amp;C2</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>Servicio-1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="5" t="str">
-        <f t="shared" ref="D3:D4" si="0">B3&amp;"-"&amp;C3</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="B3" s="1" t="str">
+        <f>TipoNotificacion!C3</f>
+        <v>Transaccional</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="10">
         <v>2</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="E3" s="5" t="str">
+        <f>B3&amp;"-"&amp;D3</f>
+        <v>Transaccional-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8289A3A7-7531-477F-85EF-0168D7D6D3E4}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="5" t="str">
+        <f>B2</f>
+        <v>Servicio</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <f>B3</f>
+        <v>Transaccional</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correccion Muetsreo - Servicios
</commit_message>
<xml_diff>
--- a/SpaOnline/ModeloDominio/Notificación - Muestreo Datos.xlsx
+++ b/SpaOnline/ModeloDominio/Notificación - Muestreo Datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DOO\DOO\SpaOnline\ModeloDominio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02557DC9-7983-4ED7-BA14-BBAA71CA8287}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B892EEFD-FEFF-4CCE-BEF6-840F90B3EEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo de Dominio Anemico" sheetId="1" r:id="rId1"/>
@@ -189,9 +189,6 @@
     <t>Combinación unica</t>
   </si>
   <si>
-    <t>Mesaje</t>
-  </si>
-  <si>
     <t>La reserva ha sido realizada exitosamente</t>
   </si>
   <si>
@@ -199,6 +196,9 @@
   </si>
   <si>
     <t>Le adjuntamos su factura emitida</t>
+  </si>
+  <si>
+    <t>Mensaje</t>
   </si>
 </sst>
 </file>
@@ -781,7 +781,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D92343-C7F8-498A-9249-704487594109}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -879,8 +879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952BDDC5-1485-4BC4-A31B-18839936F54D}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,7 +904,7 @@
         <v>32</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>33</v>
@@ -926,7 +926,7 @@
         <v>martina.corrales@gmail.com</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>30</v>
@@ -949,7 +949,7 @@
         <v>General</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>30</v>
@@ -972,7 +972,7 @@
         <v>lucrecia.gomez@hotmail.com</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>31</v>

</xml_diff>